<commit_message>
re-analysis with AFO v1.0 data
</commit_message>
<xml_diff>
--- a/AFO_field_data_exploration_22020331.xlsx
+++ b/AFO_field_data_exploration_22020331.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="r_10m" sheetId="1" r:id="rId1"/>
     <sheet name="r_30m" sheetId="2" r:id="rId2"/>
     <sheet name="r_10m_by_site" sheetId="3" r:id="rId3"/>
+    <sheet name="r_10m_1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="36">
   <si>
     <t>elev_cov</t>
   </si>
@@ -93,6 +94,42 @@
   </si>
   <si>
     <t>AFO (n = 159)</t>
+  </si>
+  <si>
+    <t>litter_d_m</t>
+  </si>
+  <si>
+    <t>litter_cov</t>
+  </si>
+  <si>
+    <t>litter_load</t>
+  </si>
+  <si>
+    <t>ns_h_m</t>
+  </si>
+  <si>
+    <t>ns_cov</t>
+  </si>
+  <si>
+    <t>elev_h_m</t>
+  </si>
+  <si>
+    <t>elev_load</t>
+  </si>
+  <si>
+    <t>bark_load</t>
+  </si>
+  <si>
+    <t>canopy_h_m</t>
+  </si>
+  <si>
+    <t>canopy_cov_m</t>
+  </si>
+  <si>
+    <t>AFO  v1 (n =159)</t>
+  </si>
+  <si>
+    <t>AFO beta (n = 159)</t>
   </si>
 </sst>
 </file>
@@ -323,7 +360,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="9">
     <dxf>
       <font>
         <b/>
@@ -424,19 +461,13 @@
       <font>
         <b/>
         <i val="0"/>
+        <strike val="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB9B9"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -725,13 +756,13 @@
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="9" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="9" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
@@ -743,7 +774,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="49.5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" ht="50.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -772,7 +803,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -801,7 +832,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -830,7 +861,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -859,7 +890,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
@@ -888,7 +919,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
@@ -917,7 +948,7 @@
         <v>-0.04</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -946,7 +977,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
@@ -975,7 +1006,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
@@ -1004,7 +1035,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -1033,7 +1064,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -1062,7 +1093,7 @@
         <v>-0.04</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
@@ -1093,7 +1124,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:I13">
-    <cfRule type="top10" dxfId="7" priority="1" rank="10"/>
+    <cfRule type="top10" dxfId="8" priority="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1108,13 +1139,13 @@
       <selection activeCell="M13" sqref="A1:M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="13" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="13" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" ht="24.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="10"/>
       <c r="B1" s="13" t="s">
         <v>20</v>
@@ -1133,7 +1164,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="49.5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:13" ht="50.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
@@ -1174,7 +1205,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>11</v>
       </c>
@@ -1215,7 +1246,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>12</v>
       </c>
@@ -1256,7 +1287,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
@@ -1297,7 +1328,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>14</v>
       </c>
@@ -1338,7 +1369,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>15</v>
       </c>
@@ -1379,7 +1410,7 @@
         <v>-0.04</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>16</v>
       </c>
@@ -1420,7 +1451,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>0</v>
       </c>
@@ -1461,7 +1492,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>17</v>
       </c>
@@ -1502,7 +1533,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>18</v>
       </c>
@@ -1543,7 +1574,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>5</v>
       </c>
@@ -1584,7 +1615,7 @@
         <v>-0.03</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>19</v>
       </c>
@@ -1627,10 +1658,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:G13">
-    <cfRule type="top10" dxfId="6" priority="4" rank="10"/>
+    <cfRule type="top10" dxfId="7" priority="4" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:M13">
-    <cfRule type="top10" dxfId="5" priority="6" rank="10"/>
+    <cfRule type="top10" dxfId="6" priority="6" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1641,17 +1672,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="13" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="13" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="25.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:22" ht="24.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="10"/>
       <c r="B1" s="13" t="s">
         <v>23</v>
@@ -1678,7 +1709,7 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="1:22" ht="49.5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:22" ht="50.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
@@ -1728,7 +1759,7 @@
       <c r="U2" s="7"/>
       <c r="V2" s="7"/>
     </row>
-    <row r="3" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>11</v>
       </c>
@@ -1778,7 +1809,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
     </row>
-    <row r="4" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>12</v>
       </c>
@@ -1828,7 +1859,7 @@
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
     </row>
-    <row r="5" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
@@ -1878,7 +1909,7 @@
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
     </row>
-    <row r="6" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>14</v>
       </c>
@@ -1928,7 +1959,7 @@
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
     </row>
-    <row r="7" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>15</v>
       </c>
@@ -1978,7 +2009,7 @@
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
     </row>
-    <row r="8" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>16</v>
       </c>
@@ -2028,7 +2059,7 @@
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
     </row>
-    <row r="9" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>0</v>
       </c>
@@ -2078,7 +2109,7 @@
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
     </row>
-    <row r="10" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>17</v>
       </c>
@@ -2128,7 +2159,7 @@
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
     </row>
-    <row r="11" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>18</v>
       </c>
@@ -2178,7 +2209,7 @@
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
     </row>
-    <row r="12" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>5</v>
       </c>
@@ -2228,7 +2259,7 @@
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
     </row>
-    <row r="13" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>19</v>
       </c>
@@ -2280,13 +2311,922 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="O3:V13">
-    <cfRule type="top10" dxfId="4" priority="3" rank="10"/>
+    <cfRule type="top10" dxfId="5" priority="3" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:G13">
-    <cfRule type="top10" dxfId="3" priority="1" rank="10"/>
+    <cfRule type="top10" dxfId="4" priority="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:M13">
-    <cfRule type="top10" dxfId="2" priority="2" rank="10"/>
+    <cfRule type="top10" dxfId="3" priority="2" rank="10"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="13" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="24.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="10"/>
+      <c r="B1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+    </row>
+    <row r="2" spans="1:22" ht="50.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="9"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+    </row>
+    <row r="3" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="16">
+        <v>0.31</v>
+      </c>
+      <c r="C3" s="17">
+        <v>0.49</v>
+      </c>
+      <c r="D3" s="16">
+        <v>0.23</v>
+      </c>
+      <c r="E3" s="16">
+        <v>0.49</v>
+      </c>
+      <c r="F3" s="16">
+        <v>0.51</v>
+      </c>
+      <c r="G3" s="16">
+        <v>0.65</v>
+      </c>
+      <c r="H3" s="18">
+        <v>0.47</v>
+      </c>
+      <c r="I3" s="19">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="J3" s="18">
+        <v>-0.06</v>
+      </c>
+      <c r="K3" s="18">
+        <v>0.52</v>
+      </c>
+      <c r="L3" s="18">
+        <v>0.2</v>
+      </c>
+      <c r="M3" s="18">
+        <v>0.49</v>
+      </c>
+      <c r="N3" s="4"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+    </row>
+    <row r="4" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="20">
+        <v>0.05</v>
+      </c>
+      <c r="C4" s="20">
+        <v>0.27</v>
+      </c>
+      <c r="D4" s="20">
+        <v>0.18</v>
+      </c>
+      <c r="E4" s="20">
+        <v>0.12</v>
+      </c>
+      <c r="F4" s="20">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G4" s="20">
+        <v>0.13</v>
+      </c>
+      <c r="H4" s="21">
+        <v>0.23</v>
+      </c>
+      <c r="I4" s="21">
+        <v>0.26</v>
+      </c>
+      <c r="J4" s="21">
+        <v>0.15</v>
+      </c>
+      <c r="K4" s="21">
+        <v>0.16</v>
+      </c>
+      <c r="L4" s="21">
+        <v>0.12</v>
+      </c>
+      <c r="M4" s="21">
+        <v>0.21</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+    </row>
+    <row r="5" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="20">
+        <v>0.23</v>
+      </c>
+      <c r="C5" s="20">
+        <v>0.41</v>
+      </c>
+      <c r="D5" s="20">
+        <v>0.19</v>
+      </c>
+      <c r="E5" s="20">
+        <v>0.41</v>
+      </c>
+      <c r="F5" s="20">
+        <v>0.42</v>
+      </c>
+      <c r="G5" s="20">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H5" s="21">
+        <v>0.34</v>
+      </c>
+      <c r="I5" s="21">
+        <v>0.43</v>
+      </c>
+      <c r="J5" s="21">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="K5" s="21">
+        <v>0.42</v>
+      </c>
+      <c r="L5" s="21">
+        <v>0.19</v>
+      </c>
+      <c r="M5" s="21">
+        <v>0.4</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+    </row>
+    <row r="6" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="20">
+        <v>-0.06</v>
+      </c>
+      <c r="C6" s="20">
+        <v>-0.09</v>
+      </c>
+      <c r="D6" s="20">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="E6" s="20">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F6" s="20">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G6" s="20">
+        <v>0.05</v>
+      </c>
+      <c r="H6" s="21">
+        <v>-0.01</v>
+      </c>
+      <c r="I6" s="21">
+        <v>-0.09</v>
+      </c>
+      <c r="J6" s="21">
+        <v>-0.18</v>
+      </c>
+      <c r="K6" s="21">
+        <v>-0.02</v>
+      </c>
+      <c r="L6" s="21">
+        <v>0.06</v>
+      </c>
+      <c r="M6" s="21">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+    </row>
+    <row r="7" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="20">
+        <v>-0.18</v>
+      </c>
+      <c r="C7" s="20">
+        <v>0.02</v>
+      </c>
+      <c r="D7" s="20">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E7" s="20">
+        <v>0.08</v>
+      </c>
+      <c r="F7" s="20">
+        <v>0.06</v>
+      </c>
+      <c r="G7" s="20">
+        <v>-0.04</v>
+      </c>
+      <c r="H7" s="21">
+        <v>-0.09</v>
+      </c>
+      <c r="I7" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="J7" s="21">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K7" s="21">
+        <v>-0.16</v>
+      </c>
+      <c r="L7" s="21">
+        <v>-0.13</v>
+      </c>
+      <c r="M7" s="21">
+        <v>-0.18</v>
+      </c>
+      <c r="N7" s="4"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+    </row>
+    <row r="8" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="C8" s="20">
+        <v>0.09</v>
+      </c>
+      <c r="D8" s="20">
+        <v>-0.04</v>
+      </c>
+      <c r="E8" s="20">
+        <v>0.22</v>
+      </c>
+      <c r="F8" s="20">
+        <v>0.25</v>
+      </c>
+      <c r="G8" s="20">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H8" s="21">
+        <v>0.23</v>
+      </c>
+      <c r="I8" s="21">
+        <v>0.17</v>
+      </c>
+      <c r="J8" s="21">
+        <v>-0.19</v>
+      </c>
+      <c r="K8" s="21">
+        <v>0.24</v>
+      </c>
+      <c r="L8" s="21">
+        <v>0.19</v>
+      </c>
+      <c r="M8" s="21">
+        <v>0.17</v>
+      </c>
+      <c r="N8" s="4"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+    </row>
+    <row r="9" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="20">
+        <v>0.11</v>
+      </c>
+      <c r="C9" s="20">
+        <v>0.06</v>
+      </c>
+      <c r="D9" s="20">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="E9" s="20">
+        <v>0.13</v>
+      </c>
+      <c r="F9" s="20">
+        <v>0.16</v>
+      </c>
+      <c r="G9" s="20">
+        <v>0.23</v>
+      </c>
+      <c r="H9" s="21">
+        <v>0.12</v>
+      </c>
+      <c r="I9" s="21">
+        <v>0.12</v>
+      </c>
+      <c r="J9" s="21">
+        <v>-0.12</v>
+      </c>
+      <c r="K9" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="L9" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="M9" s="21">
+        <v>0.02</v>
+      </c>
+      <c r="N9" s="4"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+    </row>
+    <row r="10" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="20">
+        <v>0.06</v>
+      </c>
+      <c r="C10" s="20">
+        <v>0</v>
+      </c>
+      <c r="D10" s="20">
+        <v>-0.18</v>
+      </c>
+      <c r="E10" s="20">
+        <v>0</v>
+      </c>
+      <c r="F10" s="20">
+        <v>0.02</v>
+      </c>
+      <c r="G10" s="20">
+        <v>0.09</v>
+      </c>
+      <c r="H10" s="21">
+        <v>0.04</v>
+      </c>
+      <c r="I10" s="21">
+        <v>0.02</v>
+      </c>
+      <c r="J10" s="21">
+        <v>-0.26</v>
+      </c>
+      <c r="K10" s="21">
+        <v>0.17</v>
+      </c>
+      <c r="L10" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="M10" s="21">
+        <v>0.06</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+    </row>
+    <row r="11" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="20">
+        <v>0</v>
+      </c>
+      <c r="C11" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="D11" s="20">
+        <v>0.17</v>
+      </c>
+      <c r="E11" s="20">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F11" s="20">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G11" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="H11" s="21">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I11" s="21">
+        <v>0.32</v>
+      </c>
+      <c r="J11" s="21">
+        <v>0.05</v>
+      </c>
+      <c r="K11" s="21">
+        <v>0.12</v>
+      </c>
+      <c r="L11" s="21">
+        <v>0.02</v>
+      </c>
+      <c r="M11" s="21">
+        <v>0.15</v>
+      </c>
+      <c r="N11" s="4"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+    </row>
+    <row r="12" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="20">
+        <v>-0.34</v>
+      </c>
+      <c r="C12" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="D12" s="20">
+        <v>0.49</v>
+      </c>
+      <c r="E12" s="20">
+        <v>-0.02</v>
+      </c>
+      <c r="F12" s="20">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="G12" s="20">
+        <v>-0.04</v>
+      </c>
+      <c r="H12" s="21">
+        <v>-0.05</v>
+      </c>
+      <c r="I12" s="21">
+        <v>0.24</v>
+      </c>
+      <c r="J12" s="21">
+        <v>0.44</v>
+      </c>
+      <c r="K12" s="21">
+        <v>-0.15</v>
+      </c>
+      <c r="L12" s="21">
+        <v>-0.4</v>
+      </c>
+      <c r="M12" s="21">
+        <v>-0.08</v>
+      </c>
+      <c r="N12" s="4"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+    </row>
+    <row r="13" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="22">
+        <v>0.42</v>
+      </c>
+      <c r="C13" s="22">
+        <v>0.42</v>
+      </c>
+      <c r="D13" s="20">
+        <v>0.26</v>
+      </c>
+      <c r="E13" s="20">
+        <v>0.53</v>
+      </c>
+      <c r="F13" s="20">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G13" s="20">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H13" s="23">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I13" s="21">
+        <v>0.54</v>
+      </c>
+      <c r="J13" s="21">
+        <v>0.08</v>
+      </c>
+      <c r="K13" s="21">
+        <v>0.63</v>
+      </c>
+      <c r="L13" s="21">
+        <v>0.21</v>
+      </c>
+      <c r="M13" s="21">
+        <v>0.64</v>
+      </c>
+      <c r="N13" s="4"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
+        <v>0.47</v>
+      </c>
+      <c r="C18">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D18">
+        <v>-0.06</v>
+      </c>
+      <c r="E18">
+        <v>0.52</v>
+      </c>
+      <c r="F18">
+        <v>0.2</v>
+      </c>
+      <c r="G18">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>0.23</v>
+      </c>
+      <c r="C19">
+        <v>0.26</v>
+      </c>
+      <c r="D19">
+        <v>0.15</v>
+      </c>
+      <c r="E19">
+        <v>0.16</v>
+      </c>
+      <c r="F19">
+        <v>0.12</v>
+      </c>
+      <c r="G19">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>0.34</v>
+      </c>
+      <c r="C20">
+        <v>0.43</v>
+      </c>
+      <c r="D20">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="E20">
+        <v>0.42</v>
+      </c>
+      <c r="F20">
+        <v>0.19</v>
+      </c>
+      <c r="G20">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21">
+        <v>-0.01</v>
+      </c>
+      <c r="C21">
+        <v>-0.09</v>
+      </c>
+      <c r="D21">
+        <v>-0.18</v>
+      </c>
+      <c r="E21">
+        <v>-0.02</v>
+      </c>
+      <c r="F21">
+        <v>0.06</v>
+      </c>
+      <c r="G21">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22">
+        <v>-0.09</v>
+      </c>
+      <c r="C22">
+        <v>0.03</v>
+      </c>
+      <c r="D22">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E22">
+        <v>-0.16</v>
+      </c>
+      <c r="F22">
+        <v>-0.13</v>
+      </c>
+      <c r="G22">
+        <v>-0.18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23">
+        <v>0.23</v>
+      </c>
+      <c r="C23">
+        <v>0.17</v>
+      </c>
+      <c r="D23">
+        <v>-0.19</v>
+      </c>
+      <c r="E23">
+        <v>0.24</v>
+      </c>
+      <c r="F23">
+        <v>0.19</v>
+      </c>
+      <c r="G23">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>0.12</v>
+      </c>
+      <c r="C24">
+        <v>0.12</v>
+      </c>
+      <c r="D24">
+        <v>-0.12</v>
+      </c>
+      <c r="E24">
+        <v>0.1</v>
+      </c>
+      <c r="F24">
+        <v>0.1</v>
+      </c>
+      <c r="G24">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25">
+        <v>0.04</v>
+      </c>
+      <c r="C25">
+        <v>0.02</v>
+      </c>
+      <c r="D25">
+        <v>-0.26</v>
+      </c>
+      <c r="E25">
+        <v>0.17</v>
+      </c>
+      <c r="F25">
+        <v>0.2</v>
+      </c>
+      <c r="G25">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C26">
+        <v>0.32</v>
+      </c>
+      <c r="D26">
+        <v>0.05</v>
+      </c>
+      <c r="E26">
+        <v>0.12</v>
+      </c>
+      <c r="F26">
+        <v>0.02</v>
+      </c>
+      <c r="G26">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27">
+        <v>-0.05</v>
+      </c>
+      <c r="C27">
+        <v>0.24</v>
+      </c>
+      <c r="D27">
+        <v>0.44</v>
+      </c>
+      <c r="E27">
+        <v>-0.15</v>
+      </c>
+      <c r="F27">
+        <v>-0.4</v>
+      </c>
+      <c r="G27">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C28">
+        <v>0.54</v>
+      </c>
+      <c r="D28">
+        <v>0.08</v>
+      </c>
+      <c r="E28">
+        <v>0.63</v>
+      </c>
+      <c r="F28">
+        <v>0.21</v>
+      </c>
+      <c r="G28">
+        <v>0.64</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="O3:V13">
+    <cfRule type="top10" dxfId="2" priority="3" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:G13">
+    <cfRule type="top10" dxfId="1" priority="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:M13">
+    <cfRule type="top10" dxfId="0" priority="2" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>